<commit_message>
bổ sung loại thiết bị khi khai báo trạm, update trạm
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/excel/Template_CAPNHAT_SITE.xlsx
+++ b/src/main/webapp/resources/excel/Template_CAPNHAT_SITE.xlsx
@@ -1,61 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\RIMS\trunk\code\RIMS\src\main\webapp\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\RIMS\source\RIMS\src\main\webapp\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{055FEB6C-905C-48FD-97C6-0E03B51BB437}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="331" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UPDATE SITE" sheetId="10" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UPDATE SITE'!$B$2:$S$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'UPDATE SITE'!$B$2:$R$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Z</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Z:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-BTS thì ghi là BTS.
-NodeB thì ghi là NodeB.
-EnodeB thì ghi là EnodeB
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="47">
   <si>
     <t>Thông tin khai sinh</t>
   </si>
@@ -187,9 +161,6 @@
     <t>Frequency Band</t>
   </si>
   <si>
-    <t>Loại NE</t>
-  </si>
-  <si>
     <t>BTS</t>
   </si>
   <si>
@@ -214,9 +185,6 @@
     <t>Micro</t>
   </si>
   <si>
-    <t>alcatel</t>
-  </si>
-  <si>
     <t>1/1/1</t>
   </si>
   <si>
@@ -248,17 +216,29 @@
   </si>
   <si>
     <t>U901</t>
+  </si>
+  <si>
+    <t>Loại thiết bị</t>
+  </si>
+  <si>
+    <t>BB5216</t>
+  </si>
+  <si>
+    <t>ERICSSON</t>
+  </si>
+  <si>
+    <t>Kết quả</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -299,16 +279,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -319,7 +292,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,21 +393,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -448,9 +427,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -467,19 +443,25 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 107" xfId="3"/>
-    <cellStyle name="Normal 2 11" xfId="4"/>
-    <cellStyle name="Normal 2 113" xfId="5"/>
-    <cellStyle name="Normal 2 119" xfId="6"/>
-    <cellStyle name="Normal 2 2 10 2" xfId="7"/>
-    <cellStyle name="Normal 2 51" xfId="8"/>
-    <cellStyle name="Normal 2 61" xfId="9"/>
-    <cellStyle name="Normal 2 70" xfId="10"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 107" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 11" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 113" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 119" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 10 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 51" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 61" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2 70" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -814,66 +796,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="19" style="4" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.875" customWidth="1"/>
-    <col min="19" max="19" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.375" customWidth="1"/>
-    <col min="22" max="22" width="9.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="24.75" customHeight="1">
-      <c r="A1" s="11"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
+    <row r="1" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="17" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
     </row>
-    <row r="2" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>24</v>
-      </c>
+    <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
@@ -884,7 +867,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
@@ -905,31 +888,31 @@
         <v>17</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>3</v>
@@ -938,19 +921,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>5</v>
@@ -962,7 +943,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>15</v>
@@ -970,48 +951,46 @@
       <c r="K3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="Q3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="T3" s="1" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="12" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
       <c r="F4" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" s="10">
         <v>12345678</v>
@@ -1020,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>15</v>
@@ -1028,43 +1007,44 @@
       <c r="K4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
+      <c r="L4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
       </c>
       <c r="O4" s="10">
-        <v>1</v>
-      </c>
-      <c r="P4" s="10">
         <v>23</v>
       </c>
+      <c r="P4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="Q4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="K1:S1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="K1:R1"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="S1:V1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
@@ -1076,12 +1056,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>